<commit_message>
Added export to Google sheets, new scouting attributes, and some enhancements to the sync behavior to exclude based on file extension
</commit_message>
<xml_diff>
--- a/ScoutingAppData/config/2019 Scouting Attributes.xlsx
+++ b/ScoutingAppData/config/2019 Scouting Attributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksthilaire/GitHub/ScoutingAppCentral/ScoutingAppData/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537B83AD-050C-8648-A6E1-AF750F1FF342}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D118A2B2-753B-5142-83AD-502BDCB6BF08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1160" windowWidth="22340" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36300" yWindow="1200" windowWidth="22340" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scouting Attributes" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -291,6 +291,24 @@
   </si>
   <si>
     <t>How_Many_Driveteams</t>
+  </si>
+  <si>
+    <t>Cargo_Rocket</t>
+  </si>
+  <si>
+    <t>Hatch_Panels_Cargo_Ship</t>
+  </si>
+  <si>
+    <t>Hatch_Panels_Rocket</t>
+  </si>
+  <si>
+    <t>Played_Defense</t>
+  </si>
+  <si>
+    <t>Is_Easily_Pushed</t>
+  </si>
+  <si>
+    <t>Cargo_Cargo_Ship</t>
   </si>
 </sst>
 </file>
@@ -744,11 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X963"/>
+  <dimension ref="A1:X969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1284,14 +1302,14 @@
       <c r="X13" s="11"/>
     </row>
     <row r="14" spans="1:24" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
-        <v>49</v>
+      <c r="A14" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>15</v>
@@ -1324,14 +1342,14 @@
       <c r="X14" s="11"/>
     </row>
     <row r="15" spans="1:24" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="17" t="s">
-        <v>44</v>
+      <c r="A15" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>15</v>
@@ -1364,14 +1382,14 @@
       <c r="X15" s="11"/>
     </row>
     <row r="16" spans="1:24" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="17" t="s">
-        <v>46</v>
+      <c r="A16" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>15</v>
@@ -1404,14 +1422,14 @@
       <c r="X16" s="11"/>
     </row>
     <row r="17" spans="1:24" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="17" t="s">
-        <v>47</v>
+      <c r="A17" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>15</v>
@@ -1451,7 +1469,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>15</v>
@@ -1491,7 +1509,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>15</v>
@@ -1531,7 +1549,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>15</v>
@@ -1571,7 +1589,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>15</v>
@@ -1603,190 +1621,190 @@
       <c r="W21" s="11"/>
       <c r="X21" s="11"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="1:24" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="14" t="s">
+      <c r="C22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="11">
         <v>1</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-    </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="H22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+    </row>
+    <row r="23" spans="1:24" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="14" t="s">
+      <c r="C23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="14"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-    </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="H23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+    </row>
+    <row r="24" spans="1:24" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="14" t="s">
+      <c r="C24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="14"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="11">
         <v>1</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-    </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="11" t="s">
+      <c r="H24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+    </row>
+    <row r="25" spans="1:24" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="C25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="14"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="11">
         <v>1</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
+      <c r="H25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="15" t="s">
-        <v>56</v>
+      <c r="A26" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="11"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="15"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -1804,28 +1822,29 @@
       <c r="X26" s="4"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="10" t="s">
-        <v>60</v>
+      <c r="A27" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="11">
         <v>0</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="5"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1843,28 +1862,29 @@
       <c r="X27" s="4"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="10" t="s">
-        <v>37</v>
+      <c r="A28" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="E28" s="14"/>
       <c r="F28" s="11">
         <v>1</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I28" s="5"/>
+      <c r="H28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="15"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1882,26 +1902,27 @@
       <c r="X28" s="4"/>
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="15" t="s">
-        <v>42</v>
+      <c r="A29" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="E29" s="14"/>
       <c r="F29" s="11">
         <v>1</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="11" t="s">
-        <v>23</v>
+      <c r="H29" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="I29" s="15"/>
       <c r="J29" s="4"/>
@@ -1921,26 +1942,27 @@
       <c r="X29" s="4"/>
     </row>
     <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="15" t="s">
-        <v>43</v>
+      <c r="A30" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="E30" s="14"/>
       <c r="F30" s="11">
         <v>1</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="11" t="s">
-        <v>23</v>
+      <c r="H30" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="I30" s="15"/>
       <c r="J30" s="4"/>
@@ -1960,26 +1982,27 @@
       <c r="X30" s="4"/>
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="15" t="s">
-        <v>58</v>
+      <c r="A31" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="E31" s="14"/>
       <c r="F31" s="11">
         <v>1</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H31" s="11" t="s">
-        <v>23</v>
+      <c r="H31" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="4"/>
@@ -2000,7 +2023,7 @@
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>20</v>
@@ -2011,14 +2034,15 @@
       <c r="D32" s="11" t="s">
         <v>15</v>
       </c>
+      <c r="E32" s="11"/>
       <c r="F32" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I32" s="15"/>
       <c r="J32" s="4"/>
@@ -2037,21 +2061,21 @@
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
     </row>
-    <row r="33" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="s">
-        <v>26</v>
+    <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F33" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>13</v>
@@ -2059,7 +2083,7 @@
       <c r="H33" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="4"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -2076,18 +2100,18 @@
       <c r="W33" s="4"/>
       <c r="X33" s="4"/>
     </row>
-    <row r="34" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
-        <v>28</v>
+    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F34" s="11">
         <v>1</v>
@@ -2096,9 +2120,9 @@
         <v>13</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="I34" s="5"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -2115,18 +2139,18 @@
       <c r="W34" s="4"/>
       <c r="X34" s="4"/>
     </row>
-    <row r="35" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="s">
-        <v>61</v>
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F35" s="11">
         <v>1</v>
@@ -2135,9 +2159,9 @@
         <v>13</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="I35" s="15"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -2154,18 +2178,18 @@
       <c r="W35" s="4"/>
       <c r="X35" s="4"/>
     </row>
-    <row r="36" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
-        <v>62</v>
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F36" s="11">
         <v>1</v>
@@ -2174,9 +2198,9 @@
         <v>13</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="I36" s="15"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -2193,18 +2217,18 @@
       <c r="W36" s="4"/>
       <c r="X36" s="4"/>
     </row>
-    <row r="37" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A37" s="13" t="s">
-        <v>79</v>
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F37" s="11">
         <v>1</v>
@@ -2213,9 +2237,9 @@
         <v>13</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="I37" s="15"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -2232,18 +2256,18 @@
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
     </row>
-    <row r="38" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
-        <v>76</v>
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F38" s="11">
         <v>1</v>
@@ -2252,9 +2276,9 @@
         <v>13</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I38" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="I38" s="15"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -2271,9 +2295,9 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
     </row>
-    <row r="39" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A39" s="13" t="s">
-        <v>80</v>
+    <row r="39" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>27</v>
@@ -2310,9 +2334,9 @@
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
     </row>
-    <row r="40" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A40" s="13" t="s">
-        <v>81</v>
+    <row r="40" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>27</v>
@@ -2349,9 +2373,9 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
     </row>
-    <row r="41" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A41" s="13" t="s">
-        <v>82</v>
+    <row r="41" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="22" t="s">
+        <v>61</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>27</v>
@@ -2388,9 +2412,9 @@
       <c r="W41" s="4"/>
       <c r="X41" s="4"/>
     </row>
-    <row r="42" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A42" s="13" t="s">
-        <v>83</v>
+    <row r="42" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>27</v>
@@ -2429,7 +2453,7 @@
     </row>
     <row r="43" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>27</v>
@@ -2468,7 +2492,7 @@
     </row>
     <row r="44" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>27</v>
@@ -2505,9 +2529,9 @@
       <c r="W44" s="4"/>
       <c r="X44" s="4"/>
     </row>
-    <row r="45" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="22" t="s">
-        <v>86</v>
+    <row r="45" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A45" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>27</v>
@@ -2544,9 +2568,9 @@
       <c r="W45" s="4"/>
       <c r="X45" s="4"/>
     </row>
-    <row r="46" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="22" t="s">
-        <v>87</v>
+    <row r="46" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A46" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>27</v>
@@ -2583,9 +2607,9 @@
       <c r="W46" s="4"/>
       <c r="X46" s="4"/>
     </row>
-    <row r="47" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="s">
-        <v>33</v>
+    <row r="47" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A47" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>27</v>
@@ -2622,9 +2646,9 @@
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
     </row>
-    <row r="48" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="22" t="s">
-        <v>75</v>
+    <row r="48" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A48" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>27</v>
@@ -2661,9 +2685,9 @@
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
     </row>
-    <row r="49" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="22" t="s">
-        <v>34</v>
+    <row r="49" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A49" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>27</v>
@@ -2702,7 +2726,7 @@
     </row>
     <row r="50" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>27</v>
@@ -2741,7 +2765,7 @@
     </row>
     <row r="51" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>27</v>
@@ -2780,7 +2804,7 @@
     </row>
     <row r="52" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>27</v>
@@ -2819,7 +2843,7 @@
     </row>
     <row r="53" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>27</v>
@@ -2858,7 +2882,7 @@
     </row>
     <row r="54" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>27</v>
@@ -2895,14 +2919,28 @@
       <c r="W54" s="4"/>
       <c r="X54" s="4"/>
     </row>
-    <row r="55" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A55" s="4"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
+    <row r="55" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="11">
+        <v>1</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -2920,14 +2958,28 @@
       <c r="W55" s="4"/>
       <c r="X55" s="4"/>
     </row>
-    <row r="56" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A56" s="4"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
+    <row r="56" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="11">
+        <v>1</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -2945,14 +2997,28 @@
       <c r="W56" s="4"/>
       <c r="X56" s="4"/>
     </row>
-    <row r="57" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A57" s="4"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
+    <row r="57" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="11">
+        <v>1</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -2970,14 +3036,28 @@
       <c r="W57" s="4"/>
       <c r="X57" s="4"/>
     </row>
-    <row r="58" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A58" s="4"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
+    <row r="58" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="11">
+        <v>1</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -2995,15 +3075,28 @@
       <c r="W58" s="4"/>
       <c r="X58" s="4"/>
     </row>
-    <row r="59" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A59" s="4"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
+    <row r="59" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="11">
+        <v>1</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -3021,15 +3114,28 @@
       <c r="W59" s="4"/>
       <c r="X59" s="4"/>
     </row>
-    <row r="60" spans="1:24" ht="14" x14ac:dyDescent="0.15">
-      <c r="A60" s="4"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
+    <row r="60" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="11">
+        <v>1</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -3052,7 +3158,6 @@
       <c r="B61" s="11"/>
       <c r="C61" s="4"/>
       <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
       <c r="F61" s="11"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
@@ -3078,7 +3183,6 @@
       <c r="B62" s="11"/>
       <c r="C62" s="4"/>
       <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
       <c r="F62" s="11"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
@@ -3104,7 +3208,6 @@
       <c r="B63" s="11"/>
       <c r="C63" s="4"/>
       <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
@@ -3130,7 +3233,6 @@
       <c r="B64" s="11"/>
       <c r="C64" s="4"/>
       <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
@@ -26525,6 +26627,162 @@
       <c r="W963" s="4"/>
       <c r="X963" s="4"/>
     </row>
+    <row r="964" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A964" s="4"/>
+      <c r="B964" s="11"/>
+      <c r="C964" s="4"/>
+      <c r="D964" s="11"/>
+      <c r="E964" s="11"/>
+      <c r="F964" s="11"/>
+      <c r="G964" s="11"/>
+      <c r="H964" s="11"/>
+      <c r="I964" s="4"/>
+      <c r="J964" s="4"/>
+      <c r="K964" s="4"/>
+      <c r="L964" s="4"/>
+      <c r="M964" s="4"/>
+      <c r="N964" s="4"/>
+      <c r="O964" s="4"/>
+      <c r="P964" s="4"/>
+      <c r="Q964" s="4"/>
+      <c r="R964" s="4"/>
+      <c r="S964" s="4"/>
+      <c r="T964" s="4"/>
+      <c r="U964" s="4"/>
+      <c r="V964" s="4"/>
+      <c r="W964" s="4"/>
+      <c r="X964" s="4"/>
+    </row>
+    <row r="965" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A965" s="4"/>
+      <c r="B965" s="11"/>
+      <c r="C965" s="4"/>
+      <c r="D965" s="11"/>
+      <c r="E965" s="11"/>
+      <c r="F965" s="11"/>
+      <c r="G965" s="11"/>
+      <c r="H965" s="11"/>
+      <c r="I965" s="4"/>
+      <c r="J965" s="4"/>
+      <c r="K965" s="4"/>
+      <c r="L965" s="4"/>
+      <c r="M965" s="4"/>
+      <c r="N965" s="4"/>
+      <c r="O965" s="4"/>
+      <c r="P965" s="4"/>
+      <c r="Q965" s="4"/>
+      <c r="R965" s="4"/>
+      <c r="S965" s="4"/>
+      <c r="T965" s="4"/>
+      <c r="U965" s="4"/>
+      <c r="V965" s="4"/>
+      <c r="W965" s="4"/>
+      <c r="X965" s="4"/>
+    </row>
+    <row r="966" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A966" s="4"/>
+      <c r="B966" s="11"/>
+      <c r="C966" s="4"/>
+      <c r="D966" s="11"/>
+      <c r="E966" s="11"/>
+      <c r="F966" s="11"/>
+      <c r="G966" s="11"/>
+      <c r="H966" s="11"/>
+      <c r="I966" s="4"/>
+      <c r="J966" s="4"/>
+      <c r="K966" s="4"/>
+      <c r="L966" s="4"/>
+      <c r="M966" s="4"/>
+      <c r="N966" s="4"/>
+      <c r="O966" s="4"/>
+      <c r="P966" s="4"/>
+      <c r="Q966" s="4"/>
+      <c r="R966" s="4"/>
+      <c r="S966" s="4"/>
+      <c r="T966" s="4"/>
+      <c r="U966" s="4"/>
+      <c r="V966" s="4"/>
+      <c r="W966" s="4"/>
+      <c r="X966" s="4"/>
+    </row>
+    <row r="967" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A967" s="4"/>
+      <c r="B967" s="11"/>
+      <c r="C967" s="4"/>
+      <c r="D967" s="11"/>
+      <c r="E967" s="11"/>
+      <c r="F967" s="11"/>
+      <c r="G967" s="11"/>
+      <c r="H967" s="11"/>
+      <c r="I967" s="4"/>
+      <c r="J967" s="4"/>
+      <c r="K967" s="4"/>
+      <c r="L967" s="4"/>
+      <c r="M967" s="4"/>
+      <c r="N967" s="4"/>
+      <c r="O967" s="4"/>
+      <c r="P967" s="4"/>
+      <c r="Q967" s="4"/>
+      <c r="R967" s="4"/>
+      <c r="S967" s="4"/>
+      <c r="T967" s="4"/>
+      <c r="U967" s="4"/>
+      <c r="V967" s="4"/>
+      <c r="W967" s="4"/>
+      <c r="X967" s="4"/>
+    </row>
+    <row r="968" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A968" s="4"/>
+      <c r="B968" s="11"/>
+      <c r="C968" s="4"/>
+      <c r="D968" s="11"/>
+      <c r="E968" s="11"/>
+      <c r="F968" s="11"/>
+      <c r="G968" s="11"/>
+      <c r="H968" s="11"/>
+      <c r="I968" s="4"/>
+      <c r="J968" s="4"/>
+      <c r="K968" s="4"/>
+      <c r="L968" s="4"/>
+      <c r="M968" s="4"/>
+      <c r="N968" s="4"/>
+      <c r="O968" s="4"/>
+      <c r="P968" s="4"/>
+      <c r="Q968" s="4"/>
+      <c r="R968" s="4"/>
+      <c r="S968" s="4"/>
+      <c r="T968" s="4"/>
+      <c r="U968" s="4"/>
+      <c r="V968" s="4"/>
+      <c r="W968" s="4"/>
+      <c r="X968" s="4"/>
+    </row>
+    <row r="969" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="A969" s="4"/>
+      <c r="B969" s="11"/>
+      <c r="C969" s="4"/>
+      <c r="D969" s="11"/>
+      <c r="E969" s="11"/>
+      <c r="F969" s="11"/>
+      <c r="G969" s="11"/>
+      <c r="H969" s="11"/>
+      <c r="I969" s="4"/>
+      <c r="J969" s="4"/>
+      <c r="K969" s="4"/>
+      <c r="L969" s="4"/>
+      <c r="M969" s="4"/>
+      <c r="N969" s="4"/>
+      <c r="O969" s="4"/>
+      <c r="P969" s="4"/>
+      <c r="Q969" s="4"/>
+      <c r="R969" s="4"/>
+      <c r="S969" s="4"/>
+      <c r="T969" s="4"/>
+      <c r="U969" s="4"/>
+      <c r="V969" s="4"/>
+      <c r="W969" s="4"/>
+      <c r="X969" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>